<commit_message>
configurable cookies for based on profile
</commit_message>
<xml_diff>
--- a/src/main/resources/gradsProfiles.xlsx
+++ b/src/main/resources/gradsProfiles.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Sumit Kumar</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t xml:space="preserve">hitanshu998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shivankshi Khandelwal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shivankshi13</t>
   </si>
 </sst>
 </file>
@@ -186,12 +192,14 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,6 +288,14 @@
       </c>
       <c r="B11" s="0" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fixed : stuck in infinite loop is username changed
</commit_message>
<xml_diff>
--- a/src/main/resources/gradsProfiles.xlsx
+++ b/src/main/resources/gradsProfiles.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Mandar Pande</t>
   </si>
   <si>
-    <t xml:space="preserve">mandarpande29</t>
+    <t xml:space="preserve">MandarPande</t>
   </si>
   <si>
     <t xml:space="preserve">Siddharth Pandey</t>
@@ -192,7 +192,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Week 34 questions and profiles updates
</commit_message>
<xml_diff>
--- a/src/main/resources/gradsProfiles.xlsx
+++ b/src/main/resources/gradsProfiles.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="525" windowWidth="28455" windowHeight="12210"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet0" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mj39GMhV5u0Bg+MFaRmvilPBkinXw=="/>
@@ -16,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Aditya Girisha</t>
   </si>
@@ -145,28 +148,39 @@
   </si>
   <si>
     <t>p3n7a90n</t>
+  </si>
+  <si>
+    <t>sayalijadhav1101</t>
+  </si>
+  <si>
+    <t>Pune University</t>
+  </si>
+  <si>
+    <t>Sayali Mohan Jadhav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="4">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
@@ -176,7 +190,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -186,40 +200,39 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -409,28 +422,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.71"/>
-    <col customWidth="1" min="2" max="2" width="18.86"/>
-    <col customWidth="1" min="3" max="3" width="8.57"/>
-    <col customWidth="1" min="4" max="4" width="34.0"/>
-    <col customWidth="1" min="5" max="6" width="8.57"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="5" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,13 +453,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="13.5" customHeight="1">
+    <row r="2" spans="1:4" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -452,13 +467,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="13.5" customHeight="1">
+    <row r="3" spans="1:4" ht="13.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -466,13 +481,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" ht="13.5" customHeight="1">
+    <row r="4" spans="1:4" ht="13.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -480,13 +495,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" ht="13.5" customHeight="1">
+    <row r="5" spans="1:4" ht="13.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -494,13 +509,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" ht="13.5" customHeight="1">
+    <row r="6" spans="1:4" ht="13.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -508,13 +523,13 @@
         <v>15</v>
       </c>
       <c r="C6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" ht="13.5" customHeight="1">
+    <row r="7" spans="1:4" ht="13.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -522,13 +537,13 @@
         <v>18</v>
       </c>
       <c r="C7" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" ht="13.5" customHeight="1">
+    <row r="8" spans="1:4" ht="13.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -536,13 +551,13 @@
         <v>20</v>
       </c>
       <c r="C8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" ht="13.5" customHeight="1">
+    <row r="9" spans="1:4" ht="13.5" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -550,13 +565,13 @@
         <v>23</v>
       </c>
       <c r="C9" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="13.5" customHeight="1">
+    <row r="10" spans="1:4" ht="13.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -564,13 +579,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" ht="13.5" customHeight="1">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -578,13 +593,13 @@
         <v>28</v>
       </c>
       <c r="C11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" ht="13.5" customHeight="1">
+    <row r="12" spans="1:4" ht="13.5" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -592,13 +607,13 @@
         <v>31</v>
       </c>
       <c r="C12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" ht="13.5" customHeight="1">
+    <row r="13" spans="1:4" ht="13.5" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -606,13 +621,13 @@
         <v>33</v>
       </c>
       <c r="C13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" ht="13.5" customHeight="1">
+    <row r="14" spans="1:4" ht="13.5" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -620,13 +635,13 @@
         <v>35</v>
       </c>
       <c r="C14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" ht="13.5" customHeight="1">
+    <row r="15" spans="1:4" ht="13.5" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -634,13 +649,13 @@
         <v>38</v>
       </c>
       <c r="C15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" ht="13.5" customHeight="1">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -648,13 +663,13 @@
         <v>40</v>
       </c>
       <c r="C16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" ht="13.5" customHeight="1">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>41</v>
       </c>
@@ -662,29 +677,40 @@
         <v>42</v>
       </c>
       <c r="C17" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" ht="13.5" customHeight="1">
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" ht="13.5" customHeight="1"/>
-    <row r="20" ht="13.5" customHeight="1"/>
-    <row r="21" ht="13.5" customHeight="1"/>
-    <row r="22" ht="13.5" customHeight="1"/>
-    <row r="23" ht="13.5" customHeight="1"/>
-    <row r="24" ht="13.5" customHeight="1"/>
-    <row r="25" ht="13.5" customHeight="1"/>
-    <row r="26" ht="13.5" customHeight="1"/>
-    <row r="27" ht="13.5" customHeight="1"/>
-    <row r="28" ht="13.5" customHeight="1"/>
-    <row r="29" ht="13.5" customHeight="1"/>
-    <row r="30" ht="13.5" customHeight="1"/>
-    <row r="31" ht="13.5" customHeight="1"/>
-    <row r="32" ht="13.5" customHeight="1"/>
+    <row r="18" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="20" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="21" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="22" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="23" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="24" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="25" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="26" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="27" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="28" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="29" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="30" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="31" spans="1:4" ht="13.5" customHeight="1"/>
+    <row r="32" spans="1:4" ht="13.5" customHeight="1"/>
     <row r="33" ht="13.5" customHeight="1"/>
     <row r="34" ht="13.5" customHeight="1"/>
     <row r="35" ht="13.5" customHeight="1"/>
@@ -1654,9 +1680,7 @@
     <row r="999" ht="13.5" customHeight="1"/>
     <row r="1000" ht="13.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>